<commit_message>
Basic Structure is ready including queues.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55649C\Documents\UiPath\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2E2FEF-4D5B-42C2-8E64-F7FFB3FC1171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -159,14 +156,56 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
+    <t>SharePointURL</t>
+  </si>
+  <si>
+    <t>URL of SharepointData Input</t>
+  </si>
+  <si>
+    <t>https://officemgmtentserv.sharepoint.com/sites/NewHireCommunication/Lists/New%20Hire%20Communication%20%20Employee%20Details/OfferLetterTestView.aspx</t>
+  </si>
+  <si>
+    <t>C:\Users\55649C\Documents\UiPath\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Dispatcher\Data\Input\OfferLetterInput.xlsx</t>
+  </si>
+  <si>
+    <t>Dummy Data for Sharepoint</t>
+  </si>
+  <si>
+    <t>OfferLetterInputExcel</t>
+  </si>
+  <si>
+    <t>OfferLetterTableName</t>
+  </si>
+  <si>
+    <t>OfferLetterList</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_NHC_OLC_Dispatcher_Queue</t>
+  </si>
+  <si>
+    <t>DEV</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_NHC_OLC_Dispatcher</t>
+  </si>
+  <si>
+    <t>NameExtractor</t>
+  </si>
+  <si>
+    <t>applicant.|(First)</t>
+  </si>
+  <si>
+    <t>EmailExtractor</t>
+  </si>
+  <si>
+    <t>Birth|(Email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -190,6 +229,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -208,21 +253,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -239,9 +289,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -279,7 +329,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -385,7 +435,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -527,7 +577,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -537,16 +587,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -585,44 +635,87 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1610,8 +1703,11 @@
     <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{3304E173-E629-4825-B4FA-E24275122099}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1623,12 +1719,12 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1665,7 +1761,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1673,18 +1769,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1708,7 +1804,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1730,7 +1826,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1741,7 +1837,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1752,53 +1848,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2782,14 +2878,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2800,7 +2896,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -3830,5 +3926,6 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tested for System Exceptions and Business Exceptions
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55649C\Documents\UiPath\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFFB3F6-76E5-4805-8916-3B6FCE509A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47AEFBCE-17C5-42ED-98CF-F35DE8CEF504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="95">
   <si>
     <t>Name</t>
   </si>
@@ -95,128 +95,220 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction succesful.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data.</t>
+  </si>
+  <si>
+    <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueFolder</t>
+  </si>
+  <si>
+    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>MaxConsecutiveSystemExceptions</t>
+  </si>
+  <si>
+    <t>ExceptionMessage_ConsecutiveErrors</t>
+  </si>
+  <si>
+    <t>RetryNumberGetTransactionItem</t>
+  </si>
+  <si>
+    <t>RetryNumberSetTransactionStatus</t>
+  </si>
+  <si>
+    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
+  </si>
+  <si>
+    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
+  </si>
+  <si>
+    <t>ShouldMarkJobAsFaulted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
+  </si>
+  <si>
+    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
+  </si>
+  <si>
+    <t>SharePointURL</t>
+  </si>
+  <si>
+    <t>URL of SharepointData Input</t>
+  </si>
+  <si>
+    <t>https://officemgmtentserv.sharepoint.com/sites/NewHireCommunication/Lists/New%20Hire%20Communication%20%20Employee%20Details/OfferLetterTestView.aspx</t>
+  </si>
+  <si>
+    <t>C:\Users\55649C\Documents\UiPath\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Dispatcher\Data\Input\OfferLetterInput.xlsx</t>
+  </si>
+  <si>
+    <t>Dummy Data for Sharepoint</t>
+  </si>
+  <si>
+    <t>OfferLetterInputExcel</t>
+  </si>
+  <si>
+    <t>OfferLetterTableName</t>
+  </si>
+  <si>
+    <t>OfferLetterList</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_NHC_OLC_Dispatcher_Queue</t>
+  </si>
+  <si>
+    <t>DEV</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_NHC_OLC_Dispatcher</t>
+  </si>
+  <si>
+    <t>NameExtractor</t>
+  </si>
+  <si>
+    <t>applicant.|(First)</t>
+  </si>
+  <si>
+    <t>EmailExtractor</t>
+  </si>
+  <si>
+    <t>Birth|(Email</t>
+  </si>
+  <si>
+    <t>NameNewLineException</t>
+  </si>
+  <si>
+    <t>Empty line found in the extracted name from the pdf file.</t>
+  </si>
+  <si>
+    <t>Number of characters found in the extracted name is less than 5.</t>
+  </si>
+  <si>
+    <t>NameInvalidException</t>
+  </si>
+  <si>
+    <t>EmailInvalidException</t>
+  </si>
+  <si>
+    <t>Extracted email is empty or not valid</t>
+  </si>
+  <si>
+    <t>Office365_AppID</t>
+  </si>
+  <si>
+    <t>Office365_TenantID</t>
+  </si>
+  <si>
+    <t>Office365_AppSecret</t>
+  </si>
+  <si>
+    <t>Shared_O365ApplicationID</t>
+  </si>
+  <si>
+    <t>Shared_O365TenantID</t>
+  </si>
+  <si>
+    <t>Shared_O365ApplicationSecret</t>
+  </si>
+  <si>
+    <t>Office 365 App ID to access Office 365 Apps using API</t>
+  </si>
+  <si>
+    <t>Office 365 Tenant ID to access Office 365 Apps using API</t>
+  </si>
+  <si>
+    <t>QueueField_PDFPath</t>
+  </si>
+  <si>
+    <t>BotMailID</t>
+  </si>
+  <si>
+    <t>karthick.sivabalasubramaniam.ctr@omes.ok.gov</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_BusinessExceptionContacts</t>
+  </si>
+  <si>
+    <t>Emails IDs to send Business Exceptions</t>
+  </si>
+  <si>
+    <t>BE_Contacts</t>
+  </si>
+  <si>
+    <t>SE_Contacts</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_SystemExceptionContacts</t>
+  </si>
+  <si>
+    <t>Emails IDs to send System Exceptions</t>
+  </si>
+  <si>
+    <t>Office 365 App Secret</t>
+  </si>
+  <si>
+    <t>BE_Subject</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_BE_01_Subject</t>
+  </si>
+  <si>
+    <t>Business Exception Generic Subject</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_BE_01_EmailBody</t>
+  </si>
+  <si>
+    <t>Business Exception Generic Body</t>
+  </si>
+  <si>
+    <t>BE_MailBody</t>
+  </si>
+  <si>
+    <t>BE_Subject1</t>
+  </si>
+  <si>
+    <t>BE_MailBody1</t>
+  </si>
+  <si>
+    <t>SE_Subject</t>
+  </si>
+  <si>
+    <t>SE_MailBody</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_SE_01_Subject</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_SE_01_EmailBody</t>
+  </si>
+  <si>
     <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction succesful.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Calling Get Transaction Data.</t>
-  </si>
-  <si>
-    <t>OrchestratorAssetFolder</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
-  </si>
-  <si>
-    <t>MaxConsecutiveSystemExceptions</t>
-  </si>
-  <si>
-    <t>ExceptionMessage_ConsecutiveErrors</t>
-  </si>
-  <si>
-    <t>RetryNumberGetTransactionItem</t>
-  </si>
-  <si>
-    <t>RetryNumberSetTransactionStatus</t>
-  </si>
-  <si>
-    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
-  </si>
-  <si>
-    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
-  </si>
-  <si>
-    <t>ShouldMarkJobAsFaulted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
-  </si>
-  <si>
-    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>SharePointURL</t>
-  </si>
-  <si>
-    <t>URL of SharepointData Input</t>
-  </si>
-  <si>
-    <t>https://officemgmtentserv.sharepoint.com/sites/NewHireCommunication/Lists/New%20Hire%20Communication%20%20Employee%20Details/OfferLetterTestView.aspx</t>
-  </si>
-  <si>
-    <t>C:\Users\55649C\Documents\UiPath\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Dispatcher\Data\Input\OfferLetterInput.xlsx</t>
-  </si>
-  <si>
-    <t>Dummy Data for Sharepoint</t>
-  </si>
-  <si>
-    <t>OfferLetterInputExcel</t>
-  </si>
-  <si>
-    <t>OfferLetterTableName</t>
-  </si>
-  <si>
-    <t>OfferLetterList</t>
-  </si>
-  <si>
-    <t>P004_SP002_090_NHC_OLC_Dispatcher_Queue</t>
-  </si>
-  <si>
-    <t>DEV</t>
-  </si>
-  <si>
-    <t>P004_SP002_090_NHC_OLC_Dispatcher</t>
-  </si>
-  <si>
-    <t>NameExtractor</t>
-  </si>
-  <si>
-    <t>applicant.|(First)</t>
-  </si>
-  <si>
-    <t>EmailExtractor</t>
-  </si>
-  <si>
-    <t>Birth|(Email</t>
-  </si>
-  <si>
-    <t>NameNewLineException</t>
-  </si>
-  <si>
-    <t>Empty line found in the extracted name from the pdf file.</t>
-  </si>
-  <si>
-    <t>Number of characters found in the extracted name is less than 5.</t>
-  </si>
-  <si>
-    <t>NameInvalidException</t>
-  </si>
-  <si>
-    <t>EmailInvalidException</t>
-  </si>
-  <si>
-    <t>Extracted email is empty or not valid</t>
+  </si>
+  <si>
+    <t>AddtoQueue</t>
   </si>
 </sst>
 </file>
@@ -275,7 +367,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -288,6 +380,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -603,18 +696,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
-    <col min="2" max="2" width="148.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="2" max="2" width="148.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -653,143 +746,219 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>93</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="29">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>45</v>
+        <v>64</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" t="s">
-        <v>47</v>
-      </c>
-    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" t="s">
-        <v>50</v>
+        <v>42</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" t="s">
         <v>54</v>
       </c>
-      <c r="B12" t="s">
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
         <v>55</v>
       </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" t="s">
-        <v>57</v>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A21" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A22" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" t="s">
-        <v>60</v>
-      </c>
-    </row>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:2" ht="14.25" customHeight="1">
       <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" t="s">
         <v>62</v>
       </c>
-      <c r="B23" t="s">
-        <v>63</v>
-      </c>
     </row>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>71</v>
+      </c>
+    </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A32" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A34" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A36" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -1740,13 +1909,16 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" xr:uid="{3304E173-E629-4825-B4FA-E24275122099}"/>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{3304E173-E629-4825-B4FA-E24275122099}"/>
+    <hyperlink ref="B17" r:id="rId2" xr:uid="{4B3BD2DF-4452-4B7F-BA54-B494AA98EB4D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1758,12 +1930,12 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1800,7 +1972,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1808,18 +1980,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1843,7 +2015,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1865,7 +2037,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1876,7 +2048,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1887,53 +2059,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2915,16 +3087,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="2" width="30.1796875" customWidth="1"/>
-    <col min="3" max="3" width="60.26953125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2935,7 +3109,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2963,10 +3137,62 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" t="s">
+        <v>79</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3961,7 +4187,6 @@
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Integrated With Sharepoint List Items
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,21 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55649C\Documents\UiPath\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FABD4BC1-1AD8-4EB9-97A6-899D647076BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525CE83C-6E9F-4C7D-A1AE-C29DC7AF9DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Assets!$A$1:$D$19</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="121">
   <si>
     <t>Name</t>
   </si>
@@ -155,18 +158,12 @@
     <t>SharePointURL</t>
   </si>
   <si>
-    <t>URL of SharepointData Input</t>
-  </si>
-  <si>
     <t>https://officemgmtentserv.sharepoint.com/sites/NewHireCommunication/Lists/New%20Hire%20Communication%20%20Employee%20Details/OfferLetterTestView.aspx</t>
   </si>
   <si>
     <t>C:\Users\55649C\Documents\UiPath\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Dispatcher\Data\Input\OfferLetterInput.xlsx</t>
   </si>
   <si>
-    <t>Dummy Data for Sharepoint</t>
-  </si>
-  <si>
     <t>OfferLetterInputExcel</t>
   </si>
   <si>
@@ -188,30 +185,18 @@
     <t>NameExtractor</t>
   </si>
   <si>
-    <t>applicant.|(First)</t>
-  </si>
-  <si>
     <t>EmailExtractor</t>
   </si>
   <si>
     <t>NameNewLineException</t>
   </si>
   <si>
-    <t>Empty line found in the extracted name from the pdf file.</t>
-  </si>
-  <si>
-    <t>Number of characters found in the extracted name is less than 5.</t>
-  </si>
-  <si>
     <t>NameInvalidException</t>
   </si>
   <si>
     <t>EmailInvalidException</t>
   </si>
   <si>
-    <t>Extracted email is empty or not valid</t>
-  </si>
-  <si>
     <t>Office365_AppID</t>
   </si>
   <si>
@@ -230,21 +215,9 @@
     <t>Shared_O365ApplicationSecret</t>
   </si>
   <si>
-    <t>Office 365 App ID to access Office 365 Apps using API</t>
-  </si>
-  <si>
-    <t>Office 365 Tenant ID to access Office 365 Apps using API</t>
-  </si>
-  <si>
-    <t>QueueField_PDFPath</t>
-  </si>
-  <si>
     <t>BotMailID</t>
   </si>
   <si>
-    <t>karthick.sivabalasubramaniam.ctr@omes.ok.gov</t>
-  </si>
-  <si>
     <t>P004_SP002_090_BusinessExceptionContacts</t>
   </si>
   <si>
@@ -269,39 +242,21 @@
     <t>BE_Subject</t>
   </si>
   <si>
-    <t>P004_SP002_090_BE_01_Subject</t>
-  </si>
-  <si>
     <t>Business Exception Generic Subject</t>
   </si>
   <si>
-    <t>P004_SP002_090_BE_01_EmailBody</t>
-  </si>
-  <si>
     <t>Business Exception Generic Body</t>
   </si>
   <si>
     <t>BE_MailBody</t>
   </si>
   <si>
-    <t>BE_Subject1</t>
-  </si>
-  <si>
-    <t>BE_MailBody1</t>
-  </si>
-  <si>
     <t>SE_Subject</t>
   </si>
   <si>
     <t>SE_MailBody</t>
   </si>
   <si>
-    <t>P004_SP002_090_SE_01_Subject</t>
-  </si>
-  <si>
-    <t>P004_SP002_090_SE_01_EmailBody</t>
-  </si>
-  <si>
     <t>OrchestratorQueueName</t>
   </si>
   <si>
@@ -311,13 +266,130 @@
     <t>P004_SP002_090_NHC_OLC_Performer_Queue</t>
   </si>
   <si>
-    <t>OtherDetailExtractor</t>
-  </si>
-  <si>
-    <t>(Maiden or Previous Name)|(Other Known Name(s), if any)</t>
-  </si>
-  <si>
-    <t>Date of Birth|(Email Address)</t>
+    <t>P004_SP002_090_NameExtractor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name Extractor Logic </t>
+  </si>
+  <si>
+    <t>P004_SP002_090_EmailExtractor</t>
+  </si>
+  <si>
+    <t>Email Extractor Logic</t>
+  </si>
+  <si>
+    <t>Other Details Extractor Logic</t>
+  </si>
+  <si>
+    <t>SsnDobExtractor</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_SsnDobExtractor</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_BotMailId</t>
+  </si>
+  <si>
+    <t>Bot's Mail ID</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>BotEnvironment</t>
+  </si>
+  <si>
+    <t>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_BE_Subject</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_BE_EmailBody</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_SE_Subject</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_SE_EmailBody</t>
+  </si>
+  <si>
+    <t>To Be Deleted</t>
+  </si>
+  <si>
+    <t>Temp</t>
+  </si>
+  <si>
+    <t>DelayTimeXS</t>
+  </si>
+  <si>
+    <t>DelayTimeSmall</t>
+  </si>
+  <si>
+    <t>DelayTimeMedium</t>
+  </si>
+  <si>
+    <t>DelayTimeLarge</t>
+  </si>
+  <si>
+    <t>DelayTimeKeys</t>
+  </si>
+  <si>
+    <t>LogInRetryCount</t>
+  </si>
+  <si>
+    <t>RuntimeLocalFolderPath</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_LocalRootFolder</t>
+  </si>
+  <si>
+    <t>O365_TenantID</t>
+  </si>
+  <si>
+    <t>O365_AppID</t>
+  </si>
+  <si>
+    <t>O365_AppSecret</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_BE_Name_NewLineException</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_BE_Name_NameInvalidException</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_BE_Email_EmailInvalidException</t>
+  </si>
+  <si>
+    <t>SharepointSiteURL</t>
+  </si>
+  <si>
+    <t>SSNRegexPattern</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_SSNRegexPattern</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_SharepointSiteURL</t>
+  </si>
+  <si>
+    <t>SharepointListFilter</t>
+  </si>
+  <si>
+    <t>SharepointList</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_SharepointListFilter</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_SharepointList</t>
+  </si>
+  <si>
+    <t>SharepointListColumns</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_SharepointListColumns</t>
   </si>
 </sst>
 </file>
@@ -376,7 +448,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -389,7 +461,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -409,9 +480,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -449,7 +520,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -555,7 +626,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -697,7 +768,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -705,10 +776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -755,10 +826,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -769,7 +840,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>30</v>
@@ -781,7 +852,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -789,192 +860,123 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" t="s">
-        <v>69</v>
-      </c>
-    </row>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
         <v>42</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" t="s">
-        <v>54</v>
-      </c>
-    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="B15" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A18" t="s">
-        <v>71</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A24" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A25" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A26" t="s">
-        <v>60</v>
-      </c>
-      <c r="B26" t="s">
-        <v>61</v>
-      </c>
-    </row>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A30" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A32" t="s">
-        <v>80</v>
-      </c>
-      <c r="B32" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A33" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B33" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A34" t="s">
-        <v>88</v>
-      </c>
-      <c r="B34" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A35" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B35" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="37" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A37" t="s">
-        <v>93</v>
-      </c>
-      <c r="B37" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A29" s="2"/>
+    </row>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A31" s="2"/>
+    </row>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="33" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="34" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="35" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="36" spans="3:3" ht="14.25" customHeight="1">
+      <c r="C36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="38" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="39" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="40" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="41" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="42" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="43" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="44" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="45" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="46" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="47" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="48" spans="3:3" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -1924,18 +1926,13 @@
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
-    <row r="1001" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1" xr:uid="{3304E173-E629-4825-B4FA-E24275122099}"/>
-    <hyperlink ref="B18" r:id="rId2" xr:uid="{4B3BD2DF-4452-4B7F-BA54-B494AA98EB4D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1944,7 +1941,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2125,12 +2122,54 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+    </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3104,17 +3143,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3156,87 +3195,302 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" t="s">
-        <v>74</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" t="s">
-        <v>86</v>
+      <c r="A3" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>84</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="C5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
         <v>51</v>
       </c>
-      <c r="D5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+      <c r="B12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20" t="s">
+        <v>114</v>
+      </c>
+      <c r="C20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>115</v>
+      </c>
+      <c r="B21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>116</v>
+      </c>
+      <c r="B22" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
+        <v>119</v>
+      </c>
+      <c r="B23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -4204,7 +4458,15 @@
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
+    <row r="1002" ht="14.25" customHeight="1"/>
   </sheetData>
+  <autoFilter ref="A1:D19" xr:uid="{00000000-0001-0000-0200-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D19">
+      <sortCondition ref="C1:C19"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Code Pre Freeze Check
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55649C\Documents\UiPath\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525CE83C-6E9F-4C7D-A1AE-C29DC7AF9DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE1E27E-617F-468D-B002-4A3A8E790A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="123">
   <si>
     <t>Name</t>
   </si>
@@ -390,6 +390,12 @@
   </si>
   <si>
     <t>P004_SP002_090_SharepointListColumns</t>
+  </si>
+  <si>
+    <t>SharepointBGVFolder</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_SharepointBGVFolder</t>
   </si>
 </sst>
 </file>
@@ -1941,7 +1947,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2127,7 +2133,7 @@
         <v>97</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
@@ -2135,7 +2141,7 @@
         <v>98</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
@@ -2143,7 +2149,7 @@
         <v>99</v>
       </c>
       <c r="B20">
-        <v>10</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
@@ -2151,7 +2157,7 @@
         <v>100</v>
       </c>
       <c r="B21">
-        <v>15</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
@@ -3146,7 +3152,7 @@
   <dimension ref="A1:Z1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3482,7 +3488,17 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>121</v>
+      </c>
+      <c r="B24" t="s">
+        <v>122</v>
+      </c>
+      <c r="C24" t="s">
+        <v>90</v>
+      </c>
+    </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Pre Freeze code - Copy to Shubham
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55649C\Documents\UiPath\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE1E27E-617F-468D-B002-4A3A8E790A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB6C0D8-D816-481F-A6D9-93627E7C0B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="127">
   <si>
     <t>Name</t>
   </si>
@@ -396,6 +396,18 @@
   </si>
   <si>
     <t>P004_SP002_090_SharepointBGVFolder</t>
+  </si>
+  <si>
+    <t>BgvFileNotFoundException</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_BE_BgvFileNotFound</t>
+  </si>
+  <si>
+    <t>BGVLocalFolderPath</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_BE_BGVLocalFolderPath</t>
   </si>
 </sst>
 </file>
@@ -3152,7 +3164,7 @@
   <dimension ref="A1:Z1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3499,8 +3511,28 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" t="s">
+        <v>124</v>
+      </c>
+      <c r="C25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B26" t="s">
+        <v>126</v>
+      </c>
+      <c r="C26" t="s">
+        <v>90</v>
+      </c>
+    </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Updated Code to handle Employee Name and updating Sharepoint item
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://officemgmtentserv-my.sharepoint.com/personal/karthick_sivabalasubramaniam_ctr_omes_ok_gov/Documents/Documents/UiPath/P004_SP002_090_NewHireCommunication_OfferLetterCreation_Dispatcher/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{D08D2FD4-9839-4998-B8BE-FBFAE203FF6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D851548-9CF9-405C-947D-D1365F6032F4}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{B68FD3A1-061F-4EFB-BA8F-36D3D8C66FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02597BCD-C44D-4310-9616-3B26444B207E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="136">
   <si>
     <t>Name</t>
   </si>
@@ -155,24 +155,6 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>SharePointURL</t>
-  </si>
-  <si>
-    <t>https://officemgmtentserv.sharepoint.com/sites/NewHireCommunication/Lists/New%20Hire%20Communication%20%20Employee%20Details/OfferLetterTestView.aspx</t>
-  </si>
-  <si>
-    <t>C:\Users\55649C\Documents\UiPath\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Dispatcher\Data\Input\OfferLetterInput.xlsx</t>
-  </si>
-  <si>
-    <t>OfferLetterInputExcel</t>
-  </si>
-  <si>
-    <t>OfferLetterTableName</t>
-  </si>
-  <si>
-    <t>OfferLetterList</t>
-  </si>
-  <si>
     <t>P004_SP002_090_NHC_OLC_Dispatcher_Queue</t>
   </si>
   <si>
@@ -317,9 +299,6 @@
     <t>To Be Deleted</t>
   </si>
   <si>
-    <t>Temp</t>
-  </si>
-  <si>
     <t>DelayTimeXS</t>
   </si>
   <si>
@@ -401,50 +380,68 @@
     <t>BgvFileNotFoundException</t>
   </si>
   <si>
-    <t>P004_SP002_090_BE_BgvFileNotFound</t>
+    <t>P004_SP002_090_USDateRegexPattern</t>
+  </si>
+  <si>
+    <t>USDateRegexPattern</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_EmailRegexPattern</t>
+  </si>
+  <si>
+    <t>EmailRegexPattern</t>
+  </si>
+  <si>
+    <t>ScreenshotLocalFolderPath</t>
+  </si>
+  <si>
+    <t>BE_Contacts_CC</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_BusinessExceptionCCContacts</t>
+  </si>
+  <si>
+    <t>SE_Contacts_CC</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_SystemExceptionCCContacts</t>
   </si>
   <si>
     <t>BGVLocalFolderPath</t>
   </si>
   <si>
-    <t>P004_SP002_090_BE_BGVLocalFolderPath</t>
-  </si>
-  <si>
-    <t>P004_SP002_090_USDateRegexPattern</t>
-  </si>
-  <si>
-    <t>USDateRegexPattern</t>
-  </si>
-  <si>
-    <t>P004_SP002_090_EmailRegexPattern</t>
-  </si>
-  <si>
-    <t>EmailRegexPattern</t>
-  </si>
-  <si>
-    <t>P004_SP002_090_BE_ScreenshotLocalFolderPath</t>
-  </si>
-  <si>
-    <t>ScreenshotLocalFolderPath</t>
-  </si>
-  <si>
-    <t>BE_Contacts_CC</t>
-  </si>
-  <si>
-    <t>P004_SP002_090_BusinessExceptionCCContacts</t>
-  </si>
-  <si>
-    <t>SE_Contacts_CC</t>
-  </si>
-  <si>
-    <t>P004_SP002_090_SystemExceptionCCContacts</t>
+    <t>P004_SP002_090_BGVLocalFolderPath</t>
+  </si>
+  <si>
+    <t>FilterListCondition</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_FilterListCondition</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_ScreenshotLocalFolderPath</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_BgvFileNotFound</t>
+  </si>
+  <si>
+    <t>ListFieldUpdateColumn</t>
+  </si>
+  <si>
+    <t>ListFieldUpdateValue</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_ListFieldUpdateColumn</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_ListFieldUpdateValue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -468,12 +465,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -492,11 +483,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -506,12 +496,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -525,6 +511,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -824,18 +814,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="148.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="2" max="2" width="148.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -874,33 +864,33 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -908,111 +898,81 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" t="s">
-        <v>96</v>
-      </c>
-    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>98</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" t="s">
-        <v>105</v>
-      </c>
-      <c r="B15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" t="s">
-        <v>106</v>
-      </c>
-      <c r="B16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A17" t="s">
-        <v>107</v>
-      </c>
-      <c r="B17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A29" s="2"/>
-    </row>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A31" s="2"/>
-    </row>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="33" spans="3:3" ht="14.25" customHeight="1"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:1" ht="14.25" customHeight="1">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="27" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:1" ht="14.25" customHeight="1">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="33" spans="3:3" ht="14.25" customHeight="1">
+      <c r="C33" t="s">
+        <v>89</v>
+      </c>
+    </row>
     <row r="34" spans="3:3" ht="14.25" customHeight="1"/>
     <row r="35" spans="3:3" ht="14.25" customHeight="1"/>
-    <row r="36" spans="3:3" ht="14.25" customHeight="1">
-      <c r="C36" t="s">
-        <v>95</v>
-      </c>
-    </row>
+    <row r="36" spans="3:3" ht="14.25" customHeight="1"/>
     <row r="37" spans="3:3" ht="14.25" customHeight="1"/>
     <row r="38" spans="3:3" ht="14.25" customHeight="1"/>
     <row r="39" spans="3:3" ht="14.25" customHeight="1"/>
@@ -1971,16 +1931,10 @@
     <row r="992" ht="14.25" customHeight="1"/>
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
-  <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1" xr:uid="{3304E173-E629-4825-B4FA-E24275122099}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1992,12 +1946,12 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2034,7 +1988,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2045,7 +1999,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -2159,7 +2113,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -2172,7 +2126,7 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B18">
         <v>5</v>
@@ -2180,7 +2134,7 @@
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B19">
         <v>15</v>
@@ -2188,7 +2142,7 @@
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B20">
         <v>60</v>
@@ -2196,7 +2150,7 @@
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B21">
         <v>120</v>
@@ -2204,7 +2158,7 @@
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B22">
         <v>0.1</v>
@@ -2212,7 +2166,7 @@
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -3193,16 +3147,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
     <col min="2" max="2" width="48" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="3" max="3" width="59.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3243,13 +3197,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -3277,364 +3231,394 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="B7" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C9" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B11" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="C11" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B12" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C12" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C13" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C14" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D14" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C15" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D15" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" t="s">
         <v>84</v>
       </c>
-      <c r="B16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C16" t="s">
-        <v>90</v>
-      </c>
       <c r="D16" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B17" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C17" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B18" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C18" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D18" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B19" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C19" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C20" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C21" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B22" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C22" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B23" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C23" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B24" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C24" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B25" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C25" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B26" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C26" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B27" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="C27" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B28" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C28" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B29" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B30" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C30" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.25" customHeight="1">
       <c r="A31" t="s">
+        <v>121</v>
+      </c>
+      <c r="B31" t="s">
+        <v>130</v>
+      </c>
+      <c r="C31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A32" t="s">
+        <v>128</v>
+      </c>
+      <c r="B32" t="s">
+        <v>129</v>
+      </c>
+      <c r="C32" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
         <v>132</v>
       </c>
-      <c r="B31" t="s">
-        <v>131</v>
-      </c>
-      <c r="C31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+      <c r="B33" t="s">
+        <v>134</v>
+      </c>
+      <c r="C33" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A34" t="s">
+        <v>133</v>
+      </c>
+      <c r="B34" t="s">
+        <v>135</v>
+      </c>
+      <c r="C34" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Added correct/updated GraphAPI reusable
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://officemgmtentserv-my.sharepoint.com/personal/karthick_sivabalasubramaniam_ctr_omes_ok_gov/Documents/Documents/UiPath/P004_SP002_090_NewHireCommunication_OfferLetterCreation_Dispatcher/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55649C\OneDrive - State of Oklahoma\Desktop\NHC_OLC_Dispatcher1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{B68FD3A1-061F-4EFB-BA8F-36D3D8C66FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02597BCD-C44D-4310-9616-3B26444B207E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD95FA1-194B-4298-8A45-8DCB4D595097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="139">
   <si>
     <t>Name</t>
   </si>
@@ -435,6 +435,15 @@
   </si>
   <si>
     <t>P004_SP002_090_ListFieldUpdateValue</t>
+  </si>
+  <si>
+    <t>DelayForSpDownlaod</t>
+  </si>
+  <si>
+    <t>00:01:00</t>
+  </si>
+  <si>
+    <t>Delay for downloading file from sharepoint format "00:01:00"</t>
   </si>
 </sst>
 </file>
@@ -486,7 +495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -496,6 +505,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,14 +523,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -558,7 +564,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -664,7 +670,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -806,7 +812,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1942,8 +1948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2173,7 +2179,17 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>136</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C25" t="s">
+        <v>138</v>
+      </c>
+    </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3147,7 +3163,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated config with shared asset
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55649C\Downloads\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FC67C6-047B-4877-944D-0A24656178C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9706587F-DE38-4F35-8C1D-B88858581185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="163">
   <si>
     <t>Name</t>
   </si>
@@ -213,18 +213,12 @@
     <t>BotMailID</t>
   </si>
   <si>
-    <t>P004_SP002_090_BusinessExceptionContacts</t>
-  </si>
-  <si>
     <t>BE_Contacts</t>
   </si>
   <si>
     <t>SE_Contacts</t>
   </si>
   <si>
-    <t>P004_SP002_090_SystemExceptionContacts</t>
-  </si>
-  <si>
     <t>Office 365 App Secret</t>
   </si>
   <si>
@@ -261,9 +255,6 @@
     <t>P004_SP002_090_SsnDobExtractor</t>
   </si>
   <si>
-    <t>P004_SP002_090_BotMailId</t>
-  </si>
-  <si>
     <t>Environment</t>
   </si>
   <si>
@@ -303,9 +294,6 @@
     <t>RuntimeLocalFolderPath</t>
   </si>
   <si>
-    <t>P004_SP002_090_LocalRootFolder</t>
-  </si>
-  <si>
     <t>O365_TenantID</t>
   </si>
   <si>
@@ -333,9 +321,6 @@
     <t>P004_SP002_090_SSNRegexPattern</t>
   </si>
   <si>
-    <t>P004_SP002_090_SharepointSiteURL</t>
-  </si>
-  <si>
     <t>SharepointListFilter</t>
   </si>
   <si>
@@ -345,9 +330,6 @@
     <t>P004_SP002_090_SharepointListFilter</t>
   </si>
   <si>
-    <t>P004_SP002_090_SharepointList</t>
-  </si>
-  <si>
     <t>SharepointListColumns</t>
   </si>
   <si>
@@ -381,15 +363,9 @@
     <t>BE_Contacts_CC</t>
   </si>
   <si>
-    <t>P004_SP002_090_BusinessExceptionCCContacts</t>
-  </si>
-  <si>
     <t>SE_Contacts_CC</t>
   </si>
   <si>
-    <t>P004_SP002_090_SystemExceptionCCContacts</t>
-  </si>
-  <si>
     <t>BGVLocalFolderPath</t>
   </si>
   <si>
@@ -412,9 +388,6 @@
   </si>
   <si>
     <t>ListFieldUpdateValue</t>
-  </si>
-  <si>
-    <t>P004_SP002_090_ListFieldUpdateColumn</t>
   </si>
   <si>
     <t>P004_SP002_090_ListFieldUpdateValue</t>
@@ -534,6 +507,33 @@
   </si>
   <si>
     <t>Orchestrator Asset main Folder</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_EmailAccount</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_SharepointURL</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_SharepointListName</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_SE_Email</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_BE_Email</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_LocalRootFolder</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_SE_EmailCC</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_BE_EmailCC</t>
+  </si>
+  <si>
+    <t>P004_Shared_090_Status_ColumnDisplayName</t>
   </si>
 </sst>
 </file>
@@ -584,12 +584,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -609,7 +615,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -626,6 +632,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Hyperlink 2" xfId="4" xr:uid="{BD6AE0E1-3D91-455E-B837-CFE37C0007ED}"/>
@@ -947,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z984"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -995,7 +1002,7 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>42</v>
@@ -1008,8 +1015,9 @@
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>43</v>
+      <c r="B3" s="2" t="str">
+        <f>Constants!B2</f>
+        <v>DEV</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>30</v>
@@ -1035,18 +1043,18 @@
         <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1055,35 +1063,35 @@
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B12" t="s">
         <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B13" t="s">
         <v>53</v>
       </c>
       <c r="C13" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B14" t="s">
         <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2067,8 +2075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2115,13 +2123,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="29">
@@ -2262,80 +2270,80 @@
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B19">
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B20">
         <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B21">
         <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B22">
         <v>120</v>
       </c>
       <c r="C22" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B23">
         <v>0.1</v>
       </c>
       <c r="C23" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B24">
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C26" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3311,8 +3319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3361,17 +3369,17 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C2" t="str">
         <f>Constants!B2</f>
         <v>DEV</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -3408,7 +3416,7 @@
         <v>DEV</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -3423,142 +3431,142 @@
         <v>DEV</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" t="s">
-        <v>87</v>
+        <v>83</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>159</v>
       </c>
       <c r="C5" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" t="s">
         <v>57</v>
       </c>
+      <c r="B6" s="8" t="s">
+        <v>158</v>
+      </c>
       <c r="C6" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B7" t="s">
-        <v>113</v>
+        <v>106</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>161</v>
       </c>
       <c r="C7" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C8" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C9" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>157</v>
       </c>
       <c r="C10" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>114</v>
-      </c>
-      <c r="B11" t="s">
-        <v>115</v>
+        <v>107</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>160</v>
       </c>
       <c r="C11" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C12" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C13" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
@@ -3566,14 +3574,14 @@
         <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C14" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
@@ -3581,59 +3589,59 @@
         <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C15" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C16" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B17" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C17" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1">
       <c r="A18" t="s">
         <v>56</v>
       </c>
-      <c r="B18" t="s">
-        <v>73</v>
+      <c r="B18" s="8" t="s">
+        <v>154</v>
       </c>
       <c r="C18" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1">
@@ -3641,7 +3649,7 @@
         <v>47</v>
       </c>
       <c r="B19" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C19" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
@@ -3656,7 +3664,7 @@
         <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C20" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
@@ -3671,7 +3679,7 @@
         <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C21" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
@@ -3683,197 +3691,197 @@
     </row>
     <row r="22" spans="1:4" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>94</v>
-      </c>
-      <c r="B22" t="s">
-        <v>97</v>
+        <v>90</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>155</v>
       </c>
       <c r="C22" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B23" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C23" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B24" t="s">
-        <v>101</v>
+        <v>94</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>156</v>
       </c>
       <c r="C24" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B25" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C25" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B26" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C26" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B27" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C27" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B28" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C28" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B29" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C29" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B30" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C30" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B31" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C31" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B32" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C32" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.25" customHeight="1">
       <c r="A33" t="s">
-        <v>122</v>
-      </c>
-      <c r="B33" t="s">
-        <v>124</v>
+        <v>114</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>162</v>
       </c>
       <c r="C33" t="str">
-        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
+        <v>DEV/P004_NewHireCommunication</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B34" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C34" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
         <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Added JR number in exception details
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55649C\Downloads\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Dispatcher\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56174C\Downloads\Bot Code Folder\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D780B0-33BC-4FAF-B513-C9B26BA0531C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA510EF-8E12-41B4-AD65-11A661881075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="166">
   <si>
     <t>Name</t>
   </si>
@@ -534,6 +534,15 @@
   </si>
   <si>
     <t>P004_Shared_090_Status_ColumnDisplayName</t>
+  </si>
+  <si>
+    <t>ListFieldUpdateValueException</t>
+  </si>
+  <si>
+    <t>ListField Update Value Exception value to added in sharepoint when any exception</t>
+  </si>
+  <si>
+    <t>P004_SP002_090_ListFieldUpdateValueException</t>
   </si>
 </sst>
 </file>
@@ -584,7 +593,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -600,6 +609,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -621,7 +636,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -640,6 +655,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Hyperlink 2" xfId="4" xr:uid="{BD6AE0E1-3D91-455E-B837-CFE37C0007ED}"/>
@@ -3327,7 +3343,7 @@
   <dimension ref="A1:Z1004"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3891,7 +3907,21 @@
         <v>151</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="35" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A35" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="B35" t="s">
+        <v>165</v>
+      </c>
+      <c r="C35" t="str">
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
+        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+      </c>
+      <c r="D35" t="s">
+        <v>164</v>
+      </c>
+    </row>
     <row r="36" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="37" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="38" spans="1:4" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Updated config values for PROD
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56174C\Downloads\Bot Code Folder\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA510EF-8E12-41B4-AD65-11A661881075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAEDF18-CA46-4CE6-BDBB-D0AD4ED6B2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -171,9 +171,6 @@
     <t>P004_SP002_090_NHC_OLC_Dispatcher_Queue</t>
   </si>
   <si>
-    <t>DEV</t>
-  </si>
-  <si>
     <t>P004_SP002_090_NHC_OLC_Dispatcher</t>
   </si>
   <si>
@@ -543,6 +540,9 @@
   </si>
   <si>
     <t>P004_SP002_090_ListFieldUpdateValueException</t>
+  </si>
+  <si>
+    <t>PROD</t>
   </si>
 </sst>
 </file>
@@ -679,9 +679,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -719,7 +719,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -825,7 +825,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -967,7 +967,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -977,7 +977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z984"/>
   <sheetViews>
-    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1025,7 +1025,7 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>42</v>
@@ -1040,7 +1040,7 @@
       </c>
       <c r="B3" s="2" t="str">
         <f>Constants!B2</f>
-        <v>DEV</v>
+        <v>PROD</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>30</v>
@@ -1052,7 +1052,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -1060,24 +1060,24 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" t="s">
         <v>65</v>
       </c>
-      <c r="B7" t="s">
-        <v>66</v>
-      </c>
       <c r="C7" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1086,35 +1086,35 @@
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2098,8 +2098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2146,13 +2146,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" t="s">
         <v>152</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="29">
@@ -2293,80 +2293,80 @@
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B19">
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B20">
         <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B21">
         <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B22">
         <v>120</v>
       </c>
       <c r="C22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B23">
         <v>0.1</v>
       </c>
       <c r="C23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B24">
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
+        <v>116</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="C26" t="s">
         <v>118</v>
-      </c>
-      <c r="C26" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3342,8 +3342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3392,17 +3392,17 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" t="str">
         <f>Constants!B2</f>
-        <v>DEV</v>
+        <v>PROD</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -3429,497 +3429,497 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" t="str">
         <f>Constants!B2</f>
-        <v>DEV</v>
+        <v>PROD</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" t="str">
         <f>Constants!B2</f>
-        <v>DEV</v>
+        <v>PROD</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C5" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
-        <v>DEV/P004_NewHireCommunication</v>
+        <v>PROD/P004_NewHireCommunication</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C6" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
-        <v>DEV/P004_NewHireCommunication</v>
+        <v>PROD/P004_NewHireCommunication</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C7" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
-        <v>DEV/P004_NewHireCommunication</v>
+        <v>PROD/P004_NewHireCommunication</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C9" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C10" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
-        <v>DEV/P004_NewHireCommunication</v>
+        <v>PROD/P004_NewHireCommunication</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C11" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
-        <v>DEV/P004_NewHireCommunication</v>
+        <v>PROD/P004_NewHireCommunication</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C12" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C13" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C15" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" t="s">
         <v>69</v>
-      </c>
-      <c r="B16" t="s">
-        <v>70</v>
       </c>
       <c r="C16" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1">
       <c r="A17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" t="s">
         <v>91</v>
-      </c>
-      <c r="B17" t="s">
-        <v>92</v>
       </c>
       <c r="C17" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C18" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
-        <v>DEV/P004_NewHireCommunication</v>
+        <v>PROD/P004_NewHireCommunication</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C19" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C20" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C21" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C22" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
-        <v>DEV/P004_NewHireCommunication</v>
+        <v>PROD/P004_NewHireCommunication</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C23" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C24" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
-        <v>DEV/P004_NewHireCommunication</v>
+        <v>PROD/P004_NewHireCommunication</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.25" customHeight="1">
       <c r="A25" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" t="s">
         <v>96</v>
-      </c>
-      <c r="B25" t="s">
-        <v>97</v>
       </c>
       <c r="C25" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.25" customHeight="1">
       <c r="A26" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" t="s">
         <v>98</v>
-      </c>
-      <c r="B26" t="s">
-        <v>99</v>
       </c>
       <c r="C26" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C27" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.25" customHeight="1">
       <c r="A28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" t="s">
         <v>108</v>
-      </c>
-      <c r="B28" t="s">
-        <v>109</v>
       </c>
       <c r="C28" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C29" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C30" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B31" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C31" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.25" customHeight="1">
       <c r="A32" t="s">
+        <v>109</v>
+      </c>
+      <c r="B32" t="s">
         <v>110</v>
-      </c>
-      <c r="B32" t="s">
-        <v>111</v>
       </c>
       <c r="C32" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.25" customHeight="1">
       <c r="A33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C33" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
-        <v>DEV/P004_NewHireCommunication</v>
+        <v>PROD/P004_NewHireCommunication</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14.25" customHeight="1">
       <c r="A34" t="s">
+        <v>114</v>
+      </c>
+      <c r="B34" t="s">
         <v>115</v>
-      </c>
-      <c r="B34" t="s">
-        <v>116</v>
       </c>
       <c r="C34" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="14.25" customHeight="1">
       <c r="A35" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B35" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C35" t="str">
         <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication/SP_002_OfferLetterCreation")</f>
-        <v>DEV/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
+        <v>PROD/P004_NewHireCommunication/SP_002_OfferLetterCreation</v>
       </c>
       <c r="D35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Config update for prod
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56174C\Downloads\Bot Code Folder\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAEDF18-CA46-4CE6-BDBB-D0AD4ED6B2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86816B6C-6FFA-40F7-9EDC-7DA3B81386A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -977,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z984"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1039,8 +1039,8 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="str">
-        <f>Constants!B2</f>
-        <v>PROD</v>
+        <f>_xlfn.CONCAT(Constants!B2,"/P004_NewHireCommunication")</f>
+        <v>PROD/P004_NewHireCommunication</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>30</v>
@@ -3342,8 +3342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Updated json file after code push to orchestrator
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\56174C\Downloads\Bot Code Folder\P004_SP002_090_NewHireCommunication_OfferLetterCreation_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86816B6C-6FFA-40F7-9EDC-7DA3B81386A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60553FD0-6401-4A5E-8F7C-76125946F67F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -679,9 +679,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -719,7 +719,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -825,7 +825,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -967,7 +967,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -977,7 +977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z984"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -2098,8 +2098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>